<commit_message>
code and data work
</commit_message>
<xml_diff>
--- a/results/author_country_extraction/sub_net/WestNileOutbreakSubData.xlsx
+++ b/results/author_country_extraction/sub_net/WestNileOutbreakSubData.xlsx
@@ -2506,8 +2506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFF74DEB-6C0B-441B-9D7F-0BFF6194066C}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>